<commit_message>
Show correct error values for certain pivot table show data as cases.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/ShowDataAsComplex.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/ShowDataAsComplex.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
   <si>
     <t>No.</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>Sum of Net Change</t>
   </si>
 </sst>
 </file>
@@ -625,6 +628,120 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B21:E31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="28">
+        <item m="1" x="25"/>
+        <item m="1" x="20"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item m="1" x="15"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item m="1" x="21"/>
+        <item m="1" x="18"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item m="1" x="8"/>
+        <item m="1" x="26"/>
+        <item m="1" x="13"/>
+        <item m="1" x="22"/>
+        <item m="1" x="19"/>
+        <item m="1" x="10"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item m="1" x="16"/>
+        <item x="3"/>
+        <item m="1" x="14"/>
+        <item m="1" x="11"/>
+        <item m="1" x="24"/>
+        <item m="1" x="23"/>
+        <item m="1" x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Net Change" fld="10" showDataAs="percentOfRow" baseField="1" baseItem="2" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1322,19 +1439,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" customWidth="1"/>
     <col min="8" max="8" width="30.42578125" customWidth="1"/>
@@ -1634,6 +1751,154 @@
       </c>
       <c r="H17" s="5"/>
     </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D23" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D25" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E25" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D26" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E26" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D29" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E29" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D30" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E30" s="5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="5">
+        <v>7.7005221041158214E-2</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0.92299477895884174</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix pivot table calculated fields that reference dates.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/ShowDataAsComplex.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/ShowDataAsComplex.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>No.</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Sum of Net Change</t>
+  </si>
+  <si>
+    <t>Sum of DateCalculatedField</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -242,11 +245,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -264,7 +272,7 @@
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:O10" sheet="data"/>
   </cacheSource>
-  <cacheFields count="14">
+  <cacheFields count="15">
     <cacheField name="No." numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -342,6 +350,7 @@
     <cacheField name="Balance at End date (prior year)" numFmtId="0">
       <sharedItems containsMixedTypes="1" containsNumber="1" minValue="0" maxValue="1486501.03"/>
     </cacheField>
+    <cacheField name="DateCalculatedField" numFmtId="0" formula="IF('Posting Date'&gt; 1/1/2016,7,1)" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -487,7 +496,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:H17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="14">
+  <pivotFields count="15">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="28">
@@ -546,6 +555,7 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="2"/>
@@ -631,7 +641,7 @@
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B21:E31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
+  <pivotFields count="15">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="28">
@@ -683,6 +693,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
@@ -733,6 +744,109 @@
   <dataFields count="1">
     <dataField name="Sum of Net Change" fld="10" showDataAs="percentOfRow" baseField="1" baseItem="2" numFmtId="10"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B37:C46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="15">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="28">
+        <item m="1" x="25"/>
+        <item m="1" x="20"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item m="1" x="15"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item m="1" x="21"/>
+        <item m="1" x="18"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item m="1" x="8"/>
+        <item m="1" x="26"/>
+        <item m="1" x="13"/>
+        <item m="1" x="22"/>
+        <item m="1" x="19"/>
+        <item m="1" x="10"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item m="1" x="16"/>
+        <item x="3"/>
+        <item m="1" x="14"/>
+        <item m="1" x="11"/>
+        <item m="1" x="24"/>
+        <item m="1" x="23"/>
+        <item m="1" x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of DateCalculatedField" fld="14" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1439,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,6 +2013,86 @@
         <v>1</v>
       </c>
     </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="7">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bug with calculated fields referencing shared item dates.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/ShowDataAsComplex.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/ShowDataAsComplex.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t>No.</t>
   </si>
@@ -233,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -246,6 +246,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,7 +271,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43558.476883217591" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="8">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43560.477248842595" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="8">
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:O10" sheet="data"/>
   </cacheSource>
@@ -327,7 +330,16 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Posting Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-06-24T00:00:00" maxDate="2017-12-11T00:00:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-06-24T00:00:00" maxDate="2017-12-11T00:00:00" count="8">
+        <d v="2016-07-01T00:00:00"/>
+        <d v="2010-06-24T00:00:00"/>
+        <d v="2016-08-26T00:00:00"/>
+        <d v="2012-05-06T00:00:00"/>
+        <d v="2014-10-22T00:00:00"/>
+        <d v="2017-12-10T00:00:00"/>
+        <d v="2012-10-18T00:00:00"/>
+        <d v="2013-10-25T00:00:00"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Indentation" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="3"/>
@@ -350,7 +362,7 @@
     <cacheField name="Balance at End date (prior year)" numFmtId="0">
       <sharedItems containsMixedTypes="1" containsNumber="1" minValue="0" maxValue="1486501.03"/>
     </cacheField>
-    <cacheField name="DateCalculatedField" numFmtId="0" formula="IF('Posting Date'&gt; 1/1/2016,7,1)" databaseField="0"/>
+    <cacheField name="DateCalculatedField" numFmtId="0" formula="IF('Posting Date'&gt; 41050,7,1)" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -369,7 +381,7 @@
     <x v="0"/>
     <s v="Both"/>
     <b v="1"/>
-    <d v="2016-07-01T00:00:00"/>
+    <x v="0"/>
     <n v="0"/>
     <s v=""/>
     <s v="Balance Sheet"/>
@@ -385,7 +397,7 @@
     <x v="0"/>
     <s v="Debit"/>
     <b v="1"/>
-    <d v="2010-06-24T00:00:00"/>
+    <x v="1"/>
     <n v="3"/>
     <s v=""/>
     <s v="Balance Sheet"/>
@@ -401,7 +413,7 @@
     <x v="0"/>
     <s v="Both"/>
     <b v="1"/>
-    <d v="2016-08-26T00:00:00"/>
+    <x v="2"/>
     <n v="2"/>
     <s v="11100..11700"/>
     <s v="Balance Sheet"/>
@@ -417,7 +429,7 @@
     <x v="1"/>
     <s v="Debit"/>
     <b v="1"/>
-    <d v="2012-05-06T00:00:00"/>
+    <x v="3"/>
     <n v="2"/>
     <s v="12000..12300"/>
     <s v="Balance Sheet"/>
@@ -433,7 +445,7 @@
     <x v="0"/>
     <s v="Credit"/>
     <b v="1"/>
-    <d v="2014-10-22T00:00:00"/>
+    <x v="4"/>
     <n v="2"/>
     <s v=""/>
     <s v="Balance Sheet"/>
@@ -449,7 +461,7 @@
     <x v="1"/>
     <s v="Debit"/>
     <b v="1"/>
-    <d v="2017-12-10T00:00:00"/>
+    <x v="5"/>
     <n v="3"/>
     <s v=""/>
     <s v="Balance Sheet"/>
@@ -465,7 +477,7 @@
     <x v="0"/>
     <s v="Debit"/>
     <b v="0"/>
-    <d v="2012-10-18T00:00:00"/>
+    <x v="6"/>
     <n v="3"/>
     <s v=""/>
     <s v="Balance Sheet"/>
@@ -481,7 +493,7 @@
     <x v="1"/>
     <s v="Credit"/>
     <b v="0"/>
-    <d v="2013-10-25T00:00:00"/>
+    <x v="7"/>
     <n v="2"/>
     <s v="13000..13400"/>
     <s v="Balance Sheet"/>
@@ -494,7 +506,91 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B37:C46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="15">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="9">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of DateCalculatedField" fld="14" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:H17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -638,8 +734,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B21:E31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -744,109 +840,6 @@
   <dataFields count="1">
     <dataField name="Sum of Net Change" fld="10" showDataAs="percentOfRow" baseField="1" baseItem="2" numFmtId="10"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B37:C46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="15">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="28">
-        <item m="1" x="25"/>
-        <item m="1" x="20"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item m="1" x="15"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item m="1" x="21"/>
-        <item m="1" x="18"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item m="1" x="8"/>
-        <item m="1" x="26"/>
-        <item m="1" x="13"/>
-        <item m="1" x="22"/>
-        <item m="1" x="19"/>
-        <item m="1" x="10"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item m="1" x="16"/>
-        <item x="3"/>
-        <item m="1" x="14"/>
-        <item m="1" x="11"/>
-        <item m="1" x="24"/>
-        <item m="1" x="23"/>
-        <item m="1" x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of DateCalculatedField" fld="14" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1122,7 +1115,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="H3" sqref="H3:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,80 +2006,96 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C37" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>30</v>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="8">
+        <v>40353</v>
       </c>
       <c r="C38" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="8">
+        <v>41035</v>
       </c>
       <c r="C39" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="8">
+        <v>41200</v>
       </c>
       <c r="C40" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>20</v>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="8">
+        <v>41572</v>
       </c>
       <c r="C41" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>34</v>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="8">
+        <v>41934</v>
       </c>
       <c r="C42" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>32</v>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="8">
+        <v>42552</v>
       </c>
       <c r="C43" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>23</v>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="8">
+        <v>42608</v>
       </c>
       <c r="C44" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>27</v>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="8">
+        <v>43079</v>
       </c>
       <c r="C45" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C46" s="7">

</xml_diff>